<commit_message>
Corrected range for colorbar and griddata
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4F5BE8-68B5-48B2-ADA6-46F36D61855C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612EDDA-94B8-4340-BB75-05B5B5E173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Wafer 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -347,14 +347,701 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>11279.502</v>
+      </c>
+      <c r="B1">
+        <v>2159.7424000000001</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11287.9521</v>
+      </c>
+      <c r="B2">
+        <v>2148.0286000000001</v>
+      </c>
+      <c r="C2">
+        <v>-1E-4</v>
+      </c>
+      <c r="D2">
+        <v>48.333300000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11264.305700000001</v>
+      </c>
+      <c r="B3">
+        <v>2156.4857999999999</v>
+      </c>
+      <c r="C3">
+        <v>-34.176900000000003</v>
+      </c>
+      <c r="D3">
+        <v>34.176600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11297.135700000001</v>
+      </c>
+      <c r="B4">
+        <v>2173.4279999999999</v>
+      </c>
+      <c r="C4">
+        <v>-48.333300000000001</v>
+      </c>
+      <c r="D4">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11251.218800000001</v>
+      </c>
+      <c r="B5">
+        <v>2176.989</v>
+      </c>
+      <c r="C5">
+        <v>-34.176600000000001</v>
+      </c>
+      <c r="D5">
+        <v>-34.176900000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11205.645500000001</v>
+      </c>
+      <c r="B6">
+        <v>2182.6685000000002</v>
+      </c>
+      <c r="C6">
+        <v>1E-4</v>
+      </c>
+      <c r="D6">
+        <v>-48.333300000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11210.6572</v>
+      </c>
+      <c r="B7">
+        <v>2175.9983000000002</v>
+      </c>
+      <c r="C7">
+        <v>34.176900000000003</v>
+      </c>
+      <c r="D7">
+        <v>-34.176600000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11215.300800000001</v>
+      </c>
+      <c r="B8">
+        <v>2163.5758999999998</v>
+      </c>
+      <c r="C8">
+        <v>48.333300000000001</v>
+      </c>
+      <c r="D8">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11246.233399999999</v>
+      </c>
+      <c r="B9">
+        <v>2141.2229000000002</v>
+      </c>
+      <c r="C9">
+        <v>34.176600000000001</v>
+      </c>
+      <c r="D9">
+        <v>34.176900000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11149.5283</v>
+      </c>
+      <c r="B10">
+        <v>2119.5524999999998</v>
+      </c>
+      <c r="C10">
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="D10">
+        <v>96.666700000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11108.200199999999</v>
+      </c>
+      <c r="B11">
+        <v>2143.5709999999999</v>
+      </c>
+      <c r="C11">
+        <v>-36.993099999999998</v>
+      </c>
+      <c r="D11">
+        <v>89.308300000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11107.0234</v>
+      </c>
+      <c r="B12">
+        <v>2167.4070000000002</v>
+      </c>
+      <c r="C12">
+        <v>-68.353899999999996</v>
+      </c>
+      <c r="D12">
+        <v>68.353399999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11141.300800000001</v>
+      </c>
+      <c r="B13">
+        <v>2175.0574000000001</v>
+      </c>
+      <c r="C13">
+        <v>-89.308499999999995</v>
+      </c>
+      <c r="D13">
+        <v>36.992400000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11195.915999999999</v>
+      </c>
+      <c r="B14">
+        <v>2180.1763000000001</v>
+      </c>
+      <c r="C14">
+        <v>-96.666700000000006</v>
+      </c>
+      <c r="D14">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11155.434600000001</v>
+      </c>
+      <c r="B15">
+        <v>2173.9485</v>
+      </c>
+      <c r="C15">
+        <v>-89.308300000000003</v>
+      </c>
+      <c r="D15">
+        <v>-36.993099999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11125.3037</v>
+      </c>
+      <c r="B16">
+        <v>2174.4250000000002</v>
+      </c>
+      <c r="C16">
+        <v>-68.353399999999993</v>
+      </c>
+      <c r="D16">
+        <v>-68.353899999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11127.815399999999</v>
+      </c>
+      <c r="B17">
+        <v>2181.9591999999998</v>
+      </c>
+      <c r="C17">
+        <v>-36.992400000000004</v>
+      </c>
+      <c r="D17">
+        <v>-89.308499999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11141.915999999999</v>
+      </c>
+      <c r="B18">
+        <v>2185.877</v>
+      </c>
+      <c r="C18">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D18">
+        <v>-96.666700000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11164.1885</v>
+      </c>
+      <c r="B19">
+        <v>2181.0288</v>
+      </c>
+      <c r="C19">
+        <v>36.993099999999998</v>
+      </c>
+      <c r="D19">
+        <v>-89.308300000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11166.6777</v>
+      </c>
+      <c r="B20">
+        <v>2185.5383000000002</v>
+      </c>
+      <c r="C20">
+        <v>68.353999999999999</v>
+      </c>
+      <c r="D20">
+        <v>-68.353399999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11170.551799999999</v>
+      </c>
+      <c r="B21">
+        <v>2176.2766000000001</v>
+      </c>
+      <c r="C21">
+        <v>89.308499999999995</v>
+      </c>
+      <c r="D21">
+        <v>-36.992400000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11135.3477</v>
+      </c>
+      <c r="B22">
+        <v>2161.6794</v>
+      </c>
+      <c r="C22">
+        <v>96.666700000000006</v>
+      </c>
+      <c r="D22">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11174.642599999999</v>
+      </c>
+      <c r="B23">
+        <v>2131.0437000000002</v>
+      </c>
+      <c r="C23">
+        <v>89.308300000000003</v>
+      </c>
+      <c r="D23">
+        <v>36.993099999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11175.5391</v>
+      </c>
+      <c r="B24">
+        <v>2107.7087000000001</v>
+      </c>
+      <c r="C24">
+        <v>68.353300000000004</v>
+      </c>
+      <c r="D24">
+        <v>68.353999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11178.743200000001</v>
+      </c>
+      <c r="B25">
+        <v>2107.0419999999999</v>
+      </c>
+      <c r="C25">
+        <v>36.992400000000004</v>
+      </c>
+      <c r="D25">
+        <v>89.308499999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11448.6504</v>
+      </c>
+      <c r="B26">
+        <v>2162.4994999999999</v>
+      </c>
+      <c r="C26">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="D26">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11424.1777</v>
+      </c>
+      <c r="B27">
+        <v>2192.3015</v>
+      </c>
+      <c r="C27">
+        <v>-37.529299999999999</v>
+      </c>
+      <c r="D27">
+        <v>140.0591</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>11378.354499999999</v>
+      </c>
+      <c r="B28">
+        <v>2211.4092000000001</v>
+      </c>
+      <c r="C28">
+        <v>-72.500399999999999</v>
+      </c>
+      <c r="D28">
+        <v>125.5735</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>11413.357400000001</v>
+      </c>
+      <c r="B29">
+        <v>2235.1399000000001</v>
+      </c>
+      <c r="C29">
+        <v>-102.5308</v>
+      </c>
+      <c r="D29">
+        <v>102.5301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>11495.0283</v>
+      </c>
+      <c r="B30">
+        <v>2251.9106000000002</v>
+      </c>
+      <c r="C30">
+        <v>-125.57389999999999</v>
+      </c>
+      <c r="D30">
+        <v>72.499600000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>11570.6445</v>
+      </c>
+      <c r="B31">
+        <v>2246.9978000000001</v>
+      </c>
+      <c r="C31">
+        <v>-140.05940000000001</v>
+      </c>
+      <c r="D31">
+        <v>37.528199999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11570.4473</v>
+      </c>
+      <c r="B32">
+        <v>2244.1084000000001</v>
+      </c>
+      <c r="C32">
+        <v>-145</v>
+      </c>
+      <c r="D32">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>11511.636699999999</v>
+      </c>
+      <c r="B33">
+        <v>2246.9004</v>
+      </c>
+      <c r="C33">
+        <v>-140.0591</v>
+      </c>
+      <c r="D33">
+        <v>-37.529299999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11498.1396</v>
+      </c>
+      <c r="B34">
+        <v>2225.9391999999998</v>
+      </c>
+      <c r="C34">
+        <v>-125.5733</v>
+      </c>
+      <c r="D34">
+        <v>-72.500399999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11503.482400000001</v>
+      </c>
+      <c r="B35">
+        <v>2222.9542999999999</v>
+      </c>
+      <c r="C35">
+        <v>-102.5301</v>
+      </c>
+      <c r="D35">
+        <v>-102.5309</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11510.9365</v>
+      </c>
+      <c r="B36">
+        <v>2234.0774000000001</v>
+      </c>
+      <c r="C36">
+        <v>-72.499399999999994</v>
+      </c>
+      <c r="D36">
+        <v>-125.57389999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>11534.043</v>
+      </c>
+      <c r="B37">
+        <v>2245.7395000000001</v>
+      </c>
+      <c r="C37">
+        <v>-37.528199999999998</v>
+      </c>
+      <c r="D37">
+        <v>-140.05940000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>11536.1494</v>
+      </c>
+      <c r="B38">
+        <v>2245.6271999999999</v>
+      </c>
+      <c r="C38">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="D38">
+        <v>-145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>11584.987300000001</v>
+      </c>
+      <c r="B39">
+        <v>2229.4652999999998</v>
+      </c>
+      <c r="C39">
+        <v>37.529299999999999</v>
+      </c>
+      <c r="D39">
+        <v>-140.0591</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>11678.375</v>
+      </c>
+      <c r="B40">
+        <v>2227.9789999999998</v>
+      </c>
+      <c r="C40">
+        <v>72.500600000000006</v>
+      </c>
+      <c r="D40">
+        <v>-125.5733</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>11615.862300000001</v>
+      </c>
+      <c r="B41">
+        <v>2235.2881000000002</v>
+      </c>
+      <c r="C41">
+        <v>102.5309</v>
+      </c>
+      <c r="D41">
+        <v>-102.5301</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>11584.9023</v>
+      </c>
+      <c r="B42">
+        <v>2236.1125000000002</v>
+      </c>
+      <c r="C42">
+        <v>125.5741</v>
+      </c>
+      <c r="D42">
+        <v>-72.499399999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>11589.239299999999</v>
+      </c>
+      <c r="B43">
+        <v>2240.4531000000002</v>
+      </c>
+      <c r="C43">
+        <v>140.05940000000001</v>
+      </c>
+      <c r="D43">
+        <v>-37.528199999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>11558.743200000001</v>
+      </c>
+      <c r="B44">
+        <v>2228.3422999999998</v>
+      </c>
+      <c r="C44">
+        <v>145</v>
+      </c>
+      <c r="D44">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>11543.6836</v>
+      </c>
+      <c r="B45">
+        <v>2192.5810999999999</v>
+      </c>
+      <c r="C45">
+        <v>140.0591</v>
+      </c>
+      <c r="D45">
+        <v>37.529299999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>11544.9229</v>
+      </c>
+      <c r="B46">
+        <v>2148.9306999999999</v>
+      </c>
+      <c r="C46">
+        <v>125.5733</v>
+      </c>
+      <c r="D46">
+        <v>72.500600000000006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>11519.543900000001</v>
+      </c>
+      <c r="B47">
+        <v>2138.7986000000001</v>
+      </c>
+      <c r="C47">
+        <v>102.5301</v>
+      </c>
+      <c r="D47">
+        <v>102.5309</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>11528.4336</v>
+      </c>
+      <c r="B48">
+        <v>2122.6401000000001</v>
+      </c>
+      <c r="C48">
+        <v>72.499399999999994</v>
+      </c>
+      <c r="D48">
+        <v>125.5741</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>11480.453100000001</v>
+      </c>
+      <c r="B49">
+        <v>2136.8867</v>
+      </c>
+      <c r="C49">
+        <v>37.528199999999998</v>
+      </c>
+      <c r="D49">
+        <v>140.05940000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
User instructions on Excel sheet
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D329AB-B0BE-4A51-832D-0A4D5D65C8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2649991-991E-4AF4-8026-89043CAF6637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample data" sheetId="1" r:id="rId1"/>
+    <sheet name="SIte 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Site 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>site 7 n/a</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -86,6 +91,126 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE487B9D-F1F8-41E6-A4ED-82647A848BB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8562975" y="9524"/>
+          <a:ext cx="3590925" cy="3619501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" b="1"/>
+            <a:t>Data </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" b="1" baseline="0"/>
+            <a:t>input format</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" baseline="0"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-SG" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" baseline="0"/>
+            <a:t>Each set of thickness measurements should be inserted into individual columns.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" u="sng" baseline="0"/>
+            <a:t>The last two columns of each spreadsheet should contain the coordinates of the datapoints: second last column for the X-coordinate, last column for the Y-coordinate. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" u="none" baseline="0"/>
+            <a:t> i.e. All data points in the same row should share the same coordinates.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-SG" sz="1100" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-SG" sz="1100" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" u="none" baseline="0"/>
+            <a:t>Please create a new sheet for data from a different test slot.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-SG" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" u="none" baseline="0"/>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-SG" sz="1100" u="none"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -351,40 +476,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>11279.502</v>
+        <v>11862.2246</v>
       </c>
       <c r="B1">
-        <v>2159.7424000000001</v>
+        <v>1407.9716000000001</v>
       </c>
       <c r="C1">
+        <v>10315.352500000001</v>
+      </c>
+      <c r="D1">
+        <v>1897.5787</v>
+      </c>
+      <c r="E1">
+        <v>-2.7521</v>
+      </c>
+      <c r="F1">
+        <v>127.9237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>9975.8603999999996</v>
+      </c>
+      <c r="B2">
+        <v>2512.6637999999998</v>
+      </c>
+      <c r="C2">
+        <v>10582.8887</v>
+      </c>
+      <c r="D2">
+        <v>1941.4996000000001</v>
+      </c>
+      <c r="E2">
+        <v>-2.7521</v>
+      </c>
+      <c r="F2">
+        <v>5.9196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11880.1602</v>
+      </c>
+      <c r="B3">
+        <v>1366.7128</v>
+      </c>
+      <c r="C3">
+        <v>10208.0664</v>
+      </c>
+      <c r="D3">
+        <v>1931.0449000000001</v>
+      </c>
+      <c r="E3">
+        <v>-75.925899999999999</v>
+      </c>
+      <c r="F3">
+        <v>103.52290000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11868.9521</v>
+      </c>
+      <c r="B4">
+        <v>1267.259</v>
+      </c>
+      <c r="C4">
+        <v>10008.992200000001</v>
+      </c>
+      <c r="D4">
+        <v>1952.1664000000001</v>
+      </c>
+      <c r="E4">
+        <v>-130.80629999999999</v>
+      </c>
+      <c r="F4">
+        <v>5.9196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11952.9072</v>
+      </c>
+      <c r="B5">
+        <v>1235.0132000000001</v>
+      </c>
+      <c r="C5">
+        <v>9918.0087999999996</v>
+      </c>
+      <c r="D5">
+        <v>1945.4878000000001</v>
+      </c>
+      <c r="E5">
+        <v>-75.925899999999999</v>
+      </c>
+      <c r="F5">
+        <v>-91.683700000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11997.059600000001</v>
+      </c>
+      <c r="B6">
+        <v>1226.4052999999999</v>
+      </c>
+      <c r="C6">
+        <v>9848.1376999999993</v>
+      </c>
+      <c r="D6">
+        <v>1946.4502</v>
+      </c>
+      <c r="E6">
+        <v>-2.7521</v>
+      </c>
+      <c r="F6">
+        <v>-116.08459999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12241.3613</v>
+      </c>
+      <c r="B7">
+        <v>951.45090000000005</v>
+      </c>
+      <c r="C7">
+        <v>12856.838900000001</v>
+      </c>
+      <c r="D7" t="s">
         <v>0</v>
       </c>
+      <c r="E7">
+        <v>107.0087</v>
+      </c>
+      <c r="F7">
+        <v>-67.282899999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9811.4531000000006</v>
+      </c>
+      <c r="B8">
+        <v>2586.3892000000001</v>
+      </c>
+      <c r="C8">
+        <v>10504.752899999999</v>
+      </c>
+      <c r="D8">
+        <v>1942.0724</v>
+      </c>
+      <c r="E8">
+        <v>131.4</v>
+      </c>
+      <c r="F8">
+        <v>5.9196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9827.3271000000004</v>
+      </c>
+      <c r="B9">
+        <v>2579.2892999999999</v>
+      </c>
+      <c r="C9">
+        <v>10507.949199999999</v>
+      </c>
+      <c r="D9">
+        <v>1930.7247</v>
+      </c>
+      <c r="E9">
+        <v>94.813000000000002</v>
+      </c>
+      <c r="F9">
+        <v>79.122100000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9925.7813000000006</v>
+      </c>
+      <c r="B10">
+        <v>2565.4185000000002</v>
+      </c>
+      <c r="C10">
+        <v>10579.3467</v>
+      </c>
+      <c r="D10">
+        <v>1944.5836999999999</v>
+      </c>
+      <c r="E10">
+        <v>-2.7521</v>
+      </c>
+      <c r="F10">
+        <v>79.122100000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9848.6288999999997</v>
+      </c>
+      <c r="B11">
+        <v>2558.9558000000002</v>
+      </c>
+      <c r="C11">
+        <v>10435.770500000001</v>
+      </c>
+      <c r="D11">
+        <v>1940.5238999999999</v>
+      </c>
+      <c r="E11">
+        <v>-63.7303</v>
+      </c>
+      <c r="F11">
+        <v>30.320399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9650.8583999999992</v>
+      </c>
+      <c r="B12">
+        <v>1203.6977999999999</v>
+      </c>
+      <c r="C12">
+        <v>12473.9385</v>
+      </c>
+      <c r="D12">
+        <v>1927.2145</v>
+      </c>
+      <c r="E12">
+        <v>-39.338999999999999</v>
+      </c>
+      <c r="F12">
+        <v>-42.882100000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9936.4267999999993</v>
+      </c>
+      <c r="B13">
+        <v>2550.4643999999998</v>
+      </c>
+      <c r="C13">
+        <v>10521.5527</v>
+      </c>
+      <c r="D13">
+        <v>1947.0851</v>
+      </c>
+      <c r="E13">
+        <v>64.323899999999995</v>
+      </c>
+      <c r="F13">
+        <v>-42.882100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9930.7304999999997</v>
+      </c>
+      <c r="B14">
+        <v>2533.71</v>
+      </c>
+      <c r="C14">
+        <v>10507.5479</v>
+      </c>
+      <c r="D14">
+        <v>1932.0363</v>
+      </c>
+      <c r="E14">
+        <v>58.226100000000002</v>
+      </c>
+      <c r="F14">
+        <v>30.320399999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC81E8F-26C5-4F17-AAE0-B0855E251F25}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>11838.1631</v>
+      </c>
+      <c r="B1">
+        <v>1248.8342</v>
+      </c>
+      <c r="C1">
+        <v>12170.887699999999</v>
+      </c>
       <c r="D1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>272.4683</v>
+      </c>
+      <c r="E1">
+        <v>-2.7521</v>
+      </c>
+      <c r="F1">
+        <v>127.9237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>11287.9521</v>
+        <v>11803.4756</v>
       </c>
       <c r="B2">
-        <v>2148.0286000000001</v>
+        <v>1287.2964999999999</v>
       </c>
       <c r="C2">
-        <v>-1E-4</v>
+        <v>11925.145500000001</v>
       </c>
       <c r="D2">
-        <v>48.333300000000001</v>
+        <v>295.64920000000001</v>
+      </c>
+      <c r="E2">
+        <v>-2.7521</v>
+      </c>
+      <c r="F2">
+        <v>5.9196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11751.800800000001</v>
+      </c>
+      <c r="B3">
+        <v>1216.865</v>
+      </c>
+      <c r="C3">
+        <v>12136.082</v>
+      </c>
+      <c r="D3">
+        <v>302.1807</v>
+      </c>
+      <c r="E3">
+        <v>-75.925899999999999</v>
+      </c>
+      <c r="F3">
+        <v>103.52290000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11730.1934</v>
+      </c>
+      <c r="B4">
+        <v>1225.2201</v>
+      </c>
+      <c r="C4">
+        <v>12082.1572</v>
+      </c>
+      <c r="D4">
+        <v>316.78429999999997</v>
+      </c>
+      <c r="E4">
+        <v>-130.80629999999999</v>
+      </c>
+      <c r="F4">
+        <v>5.9196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11746.9365</v>
+      </c>
+      <c r="B5">
+        <v>1286.2560000000001</v>
+      </c>
+      <c r="C5">
+        <v>11931.856400000001</v>
+      </c>
+      <c r="D5">
+        <v>294.17500000000001</v>
+      </c>
+      <c r="E5">
+        <v>-75.925899999999999</v>
+      </c>
+      <c r="F5">
+        <v>-91.683700000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11736.200199999999</v>
+      </c>
+      <c r="B6">
+        <v>1294.5945999999999</v>
+      </c>
+      <c r="C6">
+        <v>11860.156300000001</v>
+      </c>
+      <c r="D6">
+        <v>303.11180000000002</v>
+      </c>
+      <c r="E6">
+        <v>-2.7521</v>
+      </c>
+      <c r="F6">
+        <v>-116.08459999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9576.0946999999996</v>
+      </c>
+      <c r="B7">
+        <v>2600.9286999999999</v>
+      </c>
+      <c r="C7">
+        <v>10113.372100000001</v>
+      </c>
+      <c r="D7">
+        <v>1912.7926</v>
+      </c>
+      <c r="E7">
+        <v>107.0087</v>
+      </c>
+      <c r="F7">
+        <v>-67.282899999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11720.175800000001</v>
+      </c>
+      <c r="B8">
+        <v>1223.6074000000001</v>
+      </c>
+      <c r="C8">
+        <v>12056.5967</v>
+      </c>
+      <c r="D8">
+        <v>299.03820000000002</v>
+      </c>
+      <c r="E8">
+        <v>131.4</v>
+      </c>
+      <c r="F8">
+        <v>5.9196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9477.3906000000006</v>
+      </c>
+      <c r="B9">
+        <v>2550.1819</v>
+      </c>
+      <c r="C9">
+        <v>9992.4833999999992</v>
+      </c>
+      <c r="D9">
+        <v>1837.3816999999999</v>
+      </c>
+      <c r="E9">
+        <v>94.813000000000002</v>
+      </c>
+      <c r="F9">
+        <v>79.122100000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11779.7412</v>
+      </c>
+      <c r="B10">
+        <v>1294.6071999999999</v>
+      </c>
+      <c r="C10">
+        <v>11818.239299999999</v>
+      </c>
+      <c r="D10">
+        <v>280.62900000000002</v>
+      </c>
+      <c r="E10">
+        <v>-2.7521</v>
+      </c>
+      <c r="F10">
+        <v>79.122100000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11795.017599999999</v>
+      </c>
+      <c r="B11">
+        <v>1293.8094000000001</v>
+      </c>
+      <c r="C11">
+        <v>11859.7441</v>
+      </c>
+      <c r="D11">
+        <v>299.13159999999999</v>
+      </c>
+      <c r="E11">
+        <v>-63.7303</v>
+      </c>
+      <c r="F11">
+        <v>30.320399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11870.776400000001</v>
+      </c>
+      <c r="B12">
+        <v>1323.1706999999999</v>
+      </c>
+      <c r="C12">
+        <v>11820.786099999999</v>
+      </c>
+      <c r="D12">
+        <v>295.25909999999999</v>
+      </c>
+      <c r="E12">
+        <v>-39.338999999999999</v>
+      </c>
+      <c r="F12">
+        <v>-42.882100000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11870.8701</v>
+      </c>
+      <c r="B13">
+        <v>1301.8605</v>
+      </c>
+      <c r="C13">
+        <v>11919.8506</v>
+      </c>
+      <c r="D13">
+        <v>297.25599999999997</v>
+      </c>
+      <c r="E13">
+        <v>64.323899999999995</v>
+      </c>
+      <c r="F13">
+        <v>-42.882100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11842.127899999999</v>
+      </c>
+      <c r="B14">
+        <v>1316.8685</v>
+      </c>
+      <c r="C14">
+        <v>11762.0391</v>
+      </c>
+      <c r="D14">
+        <v>271.96269999999998</v>
+      </c>
+      <c r="E14">
+        <v>58.226100000000002</v>
+      </c>
+      <c r="F14">
+        <v>30.320399999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Excel user instructions
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C94736C-A6AF-4844-A83C-E46FC6093C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870FE334-D6EC-4923-A5B3-337443FB911B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,9 +183,12 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-SG" sz="1100" u="none" baseline="0"/>
-            <a:t> i.e. All data points in the same row should share the same coordinates.</a:t>
+            <a:t> i.e. All data points in the same row should share the same coordinates. </a:t>
           </a:r>
-          <a:endParaRPr lang="en-SG" sz="1100" u="sng" baseline="0"/>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" u="sng" baseline="0"/>
+            <a:t>Please enter the X, Y coordinates with units mm.</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-SG" sz="1100" u="sng" baseline="0"/>
@@ -479,7 +482,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Enabled settings on Excel sheets
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7EDB14-C8D1-418D-9406-304F6E84B4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E03F53A-E515-4F67-95C7-BA03B51EA4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slot 1" sheetId="4" r:id="rId1"/>
-    <sheet name="Slot 2" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>site 7 n/a</t>
   </si>
@@ -76,13 +74,34 @@
   </si>
   <si>
     <t>Plot 10</t>
+  </si>
+  <si>
+    <t>Wafer radius (mm)</t>
+  </si>
+  <si>
+    <t>Unit for X,Y coordinates</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>μm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Range of colorbar</t>
+  </si>
+  <si>
+    <t>(Range of colorbar entered should be larger than actual range of data values)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +115,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -113,26 +151,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -157,15 +285,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -180,8 +308,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8953500" y="66674"/>
-          <a:ext cx="3571875" cy="4067175"/>
+          <a:off x="8886825" y="971550"/>
+          <a:ext cx="3429000" cy="4305300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -440,7 +568,24 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Please create a new sheet for data from a different test slot.  You can do this by left clicking on a sheet name, and select "Move or Copy", then click "Create a copy" and "OK".</a:t>
+            <a:t>Please create a new sheet for data from a different test slot.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can do this by left clicking on a sheet name, and select "Move or Copy", then click "Create a copy" and "OK".</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -509,7 +654,76 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. If there's n filled columns in a Worksheet (excluding the last 2 columns containing coordinates), n images will be generated. The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -556,7 +770,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}" name="Table2" displayName="Table2" ref="A1:J55" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}" name="Table2" displayName="Table2" ref="A1:J55" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:J55" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E9F76CAA-1704-412D-B8CE-CA3B04892083}" name="Plot 1"/>
@@ -575,41 +789,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}" name="Table3" displayName="Table3" ref="K1:L55" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}" name="Table3" displayName="Table3" ref="K1:L55" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="K1:L55" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3F499068-4A8B-4502-ADE3-688C275C637A}" name="X"/>
     <tableColumn id="2" xr3:uid="{F8116DFA-5A18-4D98-ABBC-A8D5E11103E6}" name="Y"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{24DAC0C6-B2EB-4124-A643-0F1E288FC213}" name="Table27" displayName="Table27" ref="A1:J55" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:J55" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CAAA24BB-705F-4A4B-A80A-FDB35DE069CD}" name="Plot 1"/>
-    <tableColumn id="2" xr3:uid="{A96A166F-7D26-454E-B9ED-96FD4C7DABD7}" name="Plot 2"/>
-    <tableColumn id="3" xr3:uid="{AF77A07D-DF4A-4686-9EE0-2E28C11ECB6D}" name="Plot 3"/>
-    <tableColumn id="4" xr3:uid="{3B8900D9-CC21-4E17-9A17-7B58BFC8D62E}" name="Plot 4"/>
-    <tableColumn id="5" xr3:uid="{B9D10A16-796B-4AA9-A260-DB9776871A2B}" name="Plot 5"/>
-    <tableColumn id="6" xr3:uid="{5E38E4B4-BC12-4BEE-80F6-FD6663B99283}" name="Plot 6"/>
-    <tableColumn id="7" xr3:uid="{8291302C-DA66-4347-939C-89EE191B3D5C}" name="Plot 7"/>
-    <tableColumn id="8" xr3:uid="{E61E32E9-2F11-496B-BEFA-5770A03AB077}" name="Plot 8"/>
-    <tableColumn id="9" xr3:uid="{78F822B7-7C80-4961-B7E3-5888420DAF66}" name="Plot 9"/>
-    <tableColumn id="10" xr3:uid="{300152D7-FD7A-463D-BA9D-810F6F2150FE}" name="Plot 10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{64D710E8-1C44-435D-8059-F0BA971F6CC5}" name="Table38" displayName="Table38" ref="K1:L55" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="K1:L55" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D07BFDB2-8B2A-435B-90CD-8A7F952C8846}" name="X"/>
-    <tableColumn id="2" xr3:uid="{02F4CF70-11D1-47DB-BFCB-A1379C51C00D}" name="Y"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -878,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC50625A-E453-4126-B67A-263A5ACC8F11}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,9 +1073,11 @@
     <col min="1" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="12" width="11" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -928,8 +1114,14 @@
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4">
+        <v>150</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11862.2246</v>
       </c>
@@ -948,8 +1140,17 @@
       <c r="L2">
         <v>127.9237</v>
       </c>
+      <c r="N2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9975.8603999999996</v>
       </c>
@@ -968,8 +1169,15 @@
       <c r="L3">
         <v>5.9196</v>
       </c>
+      <c r="N3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11880.1602</v>
       </c>
@@ -988,8 +1196,14 @@
       <c r="L4">
         <v>103.52290000000001</v>
       </c>
+      <c r="N4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11868.9521</v>
       </c>
@@ -1009,7 +1223,7 @@
         <v>5.9196</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11952.9072</v>
       </c>
@@ -1029,7 +1243,7 @@
         <v>-91.683700000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11997.059600000001</v>
       </c>
@@ -1049,7 +1263,7 @@
         <v>-116.08459999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12241.3613</v>
       </c>
@@ -1059,7 +1273,7 @@
       <c r="C8">
         <v>12856.838900000001</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K8">
@@ -1069,7 +1283,7 @@
         <v>-67.282899999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9811.4531000000006</v>
       </c>
@@ -1089,7 +1303,7 @@
         <v>5.9196</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9827.3271000000004</v>
       </c>
@@ -1109,7 +1323,7 @@
         <v>79.122100000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9925.7813000000006</v>
       </c>
@@ -1129,7 +1343,7 @@
         <v>79.122100000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9848.6288999999997</v>
       </c>
@@ -1149,7 +1363,7 @@
         <v>30.320399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9650.8583999999992</v>
       </c>
@@ -1169,7 +1383,7 @@
         <v>-42.882100000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9936.4267999999993</v>
       </c>
@@ -1189,7 +1403,7 @@
         <v>-42.882100000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9930.7304999999997</v>
       </c>
@@ -1211,6 +1425,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{FB4092C1-549A-440B-ABF8-D4591512FD6B}">
+      <formula1>$P$2:$P$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1219,68 +1438,4 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA81F29-FE7A-42C0-BA49-A436353A8637}">
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="12" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Bugfix for range of extrapolation and position of words
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E03F53A-E515-4F67-95C7-BA03B51EA4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D973CBAE-49C3-4D01-8764-A8148534C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slot 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Slot 2" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>site 7 n/a</t>
   </si>
@@ -76,6 +77,12 @@
     <t>Plot 10</t>
   </si>
   <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
     <t>Wafer radius (mm)</t>
   </si>
   <si>
@@ -94,7 +101,16 @@
     <t>Range of colorbar</t>
   </si>
   <si>
+    <t>Auto</t>
+  </si>
+  <si>
     <t>(Range of colorbar entered should be larger than actual range of data values)</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Hi2</t>
   </si>
 </sst>
 </file>
@@ -235,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,11 +272,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -769,8 +792,497 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687D2300-2B01-4D81-B092-1E5A5EF88834}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886825" y="981075"/>
+          <a:ext cx="3429000" cy="4305300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:shade val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Data input format</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Each set of data points for a plot should be inserted into individual columns.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The "X", "Y" columns should contain the coordinates of the datapoints. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> i.e. All data points in the same row should share the same coordinates. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please enter the X, Y coordinates with units mm.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please create a new sheet for data from a different test slot.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can do this by left clicking on a sheet name, and select "Move or Copy", then click "Create a copy" and "OK".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can rename the columns in the first row and the new names will be used in image namings. </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}" name="Table2" displayName="Table2" ref="A1:J55" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}" name="Table2" displayName="Table2" ref="A1:J55" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:J55" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E9F76CAA-1704-412D-B8CE-CA3B04892083}" name="Plot 1"/>
@@ -789,11 +1301,41 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}" name="Table3" displayName="Table3" ref="K1:L55" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}" name="Table3" displayName="Table3" ref="K1:L55" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="K1:L55" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3F499068-4A8B-4502-ADE3-688C275C637A}" name="X"/>
     <tableColumn id="2" xr3:uid="{F8116DFA-5A18-4D98-ABBC-A8D5E11103E6}" name="Y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{63EA718A-983D-431F-847B-6CE904B48EAC}" name="Table212" displayName="Table212" ref="A1:J161" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:J161" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{B06A5652-4273-45BF-B5E1-8E8EE2C4B32B}" name="Hi"/>
+    <tableColumn id="2" xr3:uid="{AC9C8AB1-8D4C-4FB4-8EFB-3C0184F0C16B}" name="Plot 2"/>
+    <tableColumn id="3" xr3:uid="{DBEB4D72-A830-463A-8A2F-D12D6BF6B954}" name="Plot 3"/>
+    <tableColumn id="4" xr3:uid="{509B5B0B-FE72-40C8-A074-F42BCBC3EE2D}" name="Plot 4"/>
+    <tableColumn id="5" xr3:uid="{BA5CC006-DF39-4A53-9C9B-3650A72E06DB}" name="Plot 5"/>
+    <tableColumn id="6" xr3:uid="{144A9648-C02B-468F-B296-61D208B3241A}" name="Hi2"/>
+    <tableColumn id="7" xr3:uid="{D0190320-FA9A-44B4-99C7-6D1805D13FBA}" name="Plot 7"/>
+    <tableColumn id="8" xr3:uid="{E8AEE2CA-A6D9-4BE1-9FBD-DE1F831CFECD}" name="Column1"/>
+    <tableColumn id="9" xr3:uid="{8E92826C-3BFC-4502-A174-037CED71E08E}" name="Column2"/>
+    <tableColumn id="10" xr3:uid="{DD1526E5-4B0D-4F05-98F4-066AC8B6F99D}" name="Plot 10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8CBC8320-A488-46CA-AD26-836D2847824A}" name="Table313" displayName="Table313" ref="K1:L161" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="K1:L161" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{970E6553-C0F1-4E98-9D12-24A80B3E2E54}" name="X"/>
+    <tableColumn id="2" xr3:uid="{A754B5EE-2228-40E5-B30B-7476D70FB60A}" name="Y"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1064,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC50625A-E453-4126-B67A-263A5ACC8F11}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O1" s="4">
         <v>150</v>
@@ -1141,13 +1683,13 @@
         <v>127.9237</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1170,11 +1712,13 @@
         <v>5.9196</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="P3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1197,10 +1741,10 @@
         <v>103.52290000000001</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1438,4 +1982,2346 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58ADF574-3877-422C-9DBE-63782FDF5636}">
+  <dimension ref="A1:P161"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="12" width="11" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>508.36828172640003</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="K2" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L2" s="10">
+        <v>135074.34619140599</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>506.46913551149999</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L3" s="10">
+        <v>135074.34619140599</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>507.49098546720001</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="K4" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L4" s="10">
+        <v>135074.34619140599</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>507.94784226019999</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="K5" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L5" s="10">
+        <v>135074.34619140599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>506.14143917720003</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="K6" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L6" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>506.2219809211</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="K7" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L7" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>506.14198926080002</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="K8" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L8" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>506.3368160425</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="K9" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L9" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>507.67092865030003</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="K10" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L10" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>508.06090553090002</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="K11" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L11" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>507.65969628959999</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="K12" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L12" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>507.19103347629999</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="K13" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L13" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>506.21199639129998</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="K14" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L14" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>503.53583453260001</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="K15" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L15" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>505.1798968718</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="K16" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L16" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>504.55994906519999</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="K17" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L17" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>504.68103425919998</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="K18" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L18" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>505.2765473856</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="K19" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L19" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>507.39221471899998</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="K20" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L20" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>505.68590665440001</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="K21" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L21" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>505.60833122410003</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="K22" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L22" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>507.05780156740002</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="K23" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L23" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>505.36023726989998</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="K24" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L24" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>507.29234123930001</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="K25" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L25" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>505.76881296720001</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="K26" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L26" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>507.7906963634</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="K27" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L27" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>509.83305878469997</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="K28" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L28" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>508.30575559120001</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="K29" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L29" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>505.8527186</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="K30" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L30" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>506.35430825050003</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="K31" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L31" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>507.41795592030002</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="K32" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L32" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>506.59827754510002</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="K33" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L33" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>506.7303448545</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="K34" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L34" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>506.38634828630001</v>
+      </c>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="K35" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L35" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>508.06075160419999</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="K36" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L36" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>507.14301376660001</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="K37" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L37" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>506.08612143760001</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="K38" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L38" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>504.99640320370003</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="K39" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L39" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>506.51909067150001</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="K40" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L40" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>507.4010398561</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="K41" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L41" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>505.57609722929999</v>
+      </c>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="K42" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L42" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>507.04529497419998</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="K43" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L43" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>503.82989180089999</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="K44" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L44" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>504.83838626570002</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="K45" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L45" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>506.70121251130001</v>
+      </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="K46" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L46" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>505.30617168139997</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="K47" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L47" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>508.70395182750002</v>
+      </c>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="K48" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L48" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>508.27752415650002</v>
+      </c>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="K49" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L49" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>507.97805429879998</v>
+      </c>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="K50" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L50" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>507.23137949210002</v>
+      </c>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="K51" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L51" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>505.83747482929999</v>
+      </c>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="K52" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L52" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>505.23275112610003</v>
+      </c>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="K53" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L53" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>505.55489078940002</v>
+      </c>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="K54" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L54" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
+        <v>505.75672325699998</v>
+      </c>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="K55" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L55" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>507.46174422489997</v>
+      </c>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="K56" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L56" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="10">
+        <v>505.7781708393</v>
+      </c>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="K57" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L57" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="10">
+        <v>506.29255188669998</v>
+      </c>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="K58" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L58" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>507.40917216000003</v>
+      </c>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="K59" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L59" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="10">
+        <v>507.36214164030002</v>
+      </c>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="K60" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L60" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="10">
+        <v>505.94454003829998</v>
+      </c>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="K61" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L61" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="10">
+        <v>506.26983902069998</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="K62" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L62" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
+        <v>505.38198615990001</v>
+      </c>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="K63" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L63" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="10">
+        <v>506.81426540730001</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="K64" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L64" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="10">
+        <v>505.4120314443</v>
+      </c>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="K65" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L65" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="10">
+        <v>506.89331163589998</v>
+      </c>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="K66" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L66" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="10">
+        <v>506.88526217560002</v>
+      </c>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="K67" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L67" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="10">
+        <v>508.39181327239999</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="K68" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L68" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="10">
+        <v>508.32606564060001</v>
+      </c>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="K69" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L69" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="10">
+        <v>509.49072453180003</v>
+      </c>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="K70" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L70" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="10">
+        <v>511.11256765740001</v>
+      </c>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="K71" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L71" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="10">
+        <v>507.56900084680001</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="K72" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L72" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="10">
+        <v>507.42683955669997</v>
+      </c>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="K73" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L73" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
+        <v>507.05576994</v>
+      </c>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="K74" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L74" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
+        <v>507.44634169</v>
+      </c>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="K75" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L75" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="10">
+        <v>507.53114358459999</v>
+      </c>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="K76" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L76" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="10">
+        <v>506.8724407986</v>
+      </c>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="K77" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L77" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
+        <v>507.06825752809999</v>
+      </c>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="K78" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L78" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="10">
+        <v>506.85195381509999</v>
+      </c>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="K79" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L79" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="10">
+        <v>506.26778247919998</v>
+      </c>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="K80" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L80" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="10">
+        <v>506.53828329100003</v>
+      </c>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="K81" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L81" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>507.90198703829998</v>
+      </c>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="K82" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L82" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="10">
+        <v>506.62476672420001</v>
+      </c>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="K83" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L83" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="10">
+        <v>507.40631653849999</v>
+      </c>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="K84" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L84" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="10">
+        <v>508.0877120376</v>
+      </c>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="K85" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L85" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="10">
+        <v>507.14928302499999</v>
+      </c>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="K86" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L86" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="10">
+        <v>508.1512023107</v>
+      </c>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="K87" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L87" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="10">
+        <v>507.4980302372</v>
+      </c>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="K88" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L88" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="10">
+        <v>508.28363662729998</v>
+      </c>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="K89" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L89" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="10">
+        <v>507.50816252689998</v>
+      </c>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="K90" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L90" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="10">
+        <v>507.62666497409998</v>
+      </c>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="K91" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L91" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="10">
+        <v>507.62669499899999</v>
+      </c>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="K92" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L92" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="10">
+        <v>508.87112796500003</v>
+      </c>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="K93" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L93" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="10">
+        <v>507.06661210009997</v>
+      </c>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="K94" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L94" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="10">
+        <v>507.6134279858</v>
+      </c>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="K95" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L95" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="10">
+        <v>507.13697527839997</v>
+      </c>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="K96" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L96" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="10">
+        <v>507.60699275809998</v>
+      </c>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="K97" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L97" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="10">
+        <v>507.95306041600003</v>
+      </c>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="K98" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L98" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="10">
+        <v>507.795266368</v>
+      </c>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="K99" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L99" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="10">
+        <v>507.25245776179997</v>
+      </c>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="K100" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L100" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="10">
+        <v>506.99316613830001</v>
+      </c>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="K101" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L101" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="10">
+        <v>507.46517910159997</v>
+      </c>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+      <c r="I102" s="10"/>
+      <c r="K102" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L102" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="10">
+        <v>507.89433567740002</v>
+      </c>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="K103" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L103" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="10">
+        <v>507.40430452610002</v>
+      </c>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="K104" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L104" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="10">
+        <v>506.73101552740002</v>
+      </c>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="K105" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L105" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="10">
+        <v>506.36912536009999</v>
+      </c>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="K106" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L106" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="10">
+        <v>507.10280864660001</v>
+      </c>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="K107" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L107" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108" s="10">
+        <v>505.29861237350002</v>
+      </c>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="K108" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L108" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" s="10">
+        <v>506.6675904544</v>
+      </c>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="K109" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L109" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" s="10">
+        <v>506.68239760469999</v>
+      </c>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+      <c r="K110" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L110" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="10">
+        <v>505.79287174669997</v>
+      </c>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="K111" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L111" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" s="10">
+        <v>506.20664817890002</v>
+      </c>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="K112" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L112" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="10">
+        <v>506.70521801479998</v>
+      </c>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
+      <c r="I113" s="10"/>
+      <c r="K113" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L113" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="10">
+        <v>508.84779533059998</v>
+      </c>
+      <c r="G114" s="10"/>
+      <c r="H114" s="10"/>
+      <c r="I114" s="10"/>
+      <c r="K114" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L114" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="10">
+        <v>508.86391012370001</v>
+      </c>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="K115" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L115" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="10">
+        <v>507.27215344849998</v>
+      </c>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
+      <c r="I116" s="10"/>
+      <c r="K116" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L116" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="10">
+        <v>506.39187865129998</v>
+      </c>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+      <c r="K117" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L117" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="10">
+        <v>507.10705694059999</v>
+      </c>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+      <c r="I118" s="10"/>
+      <c r="K118" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L118" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="10">
+        <v>507.69632012770001</v>
+      </c>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+      <c r="I119" s="10"/>
+      <c r="K119" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L119" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="10">
+        <v>506.62663214460002</v>
+      </c>
+      <c r="G120" s="10"/>
+      <c r="H120" s="10"/>
+      <c r="I120" s="10"/>
+      <c r="K120" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L120" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="10">
+        <v>506.06629126849998</v>
+      </c>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+      <c r="K121" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L121" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" s="10">
+        <v>507.42915641180002</v>
+      </c>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="K122" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L122" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="10">
+        <v>506.60776187900001</v>
+      </c>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="K123" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L123" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="10">
+        <v>509.18979865649999</v>
+      </c>
+      <c r="G124" s="10"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="K124" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L124" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="10">
+        <v>508.85556336209999</v>
+      </c>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="K125" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L125" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" s="10">
+        <v>508.9222274828</v>
+      </c>
+      <c r="G126" s="10"/>
+      <c r="H126" s="10"/>
+      <c r="I126" s="10"/>
+      <c r="K126" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L126" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="10">
+        <v>507.32045756999997</v>
+      </c>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="K127" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L127" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="10">
+        <v>508.67007377610003</v>
+      </c>
+      <c r="G128" s="10"/>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+      <c r="K128" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L128" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="10">
+        <v>507.69189612240001</v>
+      </c>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="K129" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L129" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" s="10">
+        <v>504.3425767448</v>
+      </c>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+      <c r="K130" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L130" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="10">
+        <v>507.48012327729998</v>
+      </c>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="K131" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L131" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="10">
+        <v>507.13903611770002</v>
+      </c>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="K132" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L132" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133" s="10">
+        <v>507.72222661759997</v>
+      </c>
+      <c r="G133" s="10"/>
+      <c r="H133" s="10"/>
+      <c r="I133" s="10"/>
+      <c r="K133" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L133" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="10">
+        <v>509.37322456700002</v>
+      </c>
+      <c r="G134" s="10"/>
+      <c r="H134" s="10"/>
+      <c r="I134" s="10"/>
+      <c r="K134" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L134" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" s="10">
+        <v>508.61913568940003</v>
+      </c>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+      <c r="K135" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L135" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="10">
+        <v>507.84549219759998</v>
+      </c>
+      <c r="G136" s="10"/>
+      <c r="H136" s="10"/>
+      <c r="I136" s="10"/>
+      <c r="K136" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L136" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="10">
+        <v>506.7125765111</v>
+      </c>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+      <c r="K137" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L137" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138" s="10">
+        <v>508.23058244020001</v>
+      </c>
+      <c r="G138" s="10"/>
+      <c r="H138" s="10"/>
+      <c r="I138" s="10"/>
+      <c r="K138" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L138" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" s="10">
+        <v>506.82398959480003</v>
+      </c>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+      <c r="K139" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L139" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="10">
+        <v>509.10760069690002</v>
+      </c>
+      <c r="G140" s="10"/>
+      <c r="H140" s="10"/>
+      <c r="I140" s="10"/>
+      <c r="K140" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L140" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" s="10">
+        <v>507.20794061459998</v>
+      </c>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
+      <c r="K141" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L141" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="10">
+        <v>508.90399061120002</v>
+      </c>
+      <c r="G142" s="10"/>
+      <c r="H142" s="10"/>
+      <c r="I142" s="10"/>
+      <c r="K142" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L142" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="10">
+        <v>508.4898106018</v>
+      </c>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+      <c r="K143" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L143" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" s="10">
+        <v>507.23381260849999</v>
+      </c>
+      <c r="G144" s="10"/>
+      <c r="H144" s="10"/>
+      <c r="I144" s="10"/>
+      <c r="K144" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L144" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" s="10">
+        <v>506.89998225990001</v>
+      </c>
+      <c r="G145" s="10"/>
+      <c r="H145" s="10"/>
+      <c r="I145" s="10"/>
+      <c r="K145" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L145" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" s="10">
+        <v>507.9829626216</v>
+      </c>
+      <c r="G146" s="10"/>
+      <c r="H146" s="10"/>
+      <c r="I146" s="10"/>
+      <c r="K146" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L146" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="10">
+        <v>506.72239559100001</v>
+      </c>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+      <c r="K147" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L147" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" s="10">
+        <v>507.12327032979999</v>
+      </c>
+      <c r="G148" s="10"/>
+      <c r="H148" s="10"/>
+      <c r="I148" s="10"/>
+      <c r="K148" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L148" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" s="10">
+        <v>506.22694080259998</v>
+      </c>
+      <c r="G149" s="10"/>
+      <c r="H149" s="10"/>
+      <c r="I149" s="10"/>
+      <c r="K149" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L149" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" s="10">
+        <v>508.38049034779999</v>
+      </c>
+      <c r="G150" s="10"/>
+      <c r="H150" s="10"/>
+      <c r="I150" s="10"/>
+      <c r="K150" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L150" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" s="10">
+        <v>508.51205468609999</v>
+      </c>
+      <c r="G151" s="10"/>
+      <c r="H151" s="10"/>
+      <c r="I151" s="10"/>
+      <c r="K151" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L151" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152" s="10">
+        <v>507.4783165019</v>
+      </c>
+      <c r="G152" s="10"/>
+      <c r="H152" s="10"/>
+      <c r="I152" s="10"/>
+      <c r="K152" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L152" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A153" s="10">
+        <v>508.47489269149997</v>
+      </c>
+      <c r="G153" s="10"/>
+      <c r="H153" s="10"/>
+      <c r="I153" s="10"/>
+      <c r="K153" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L153" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A154" s="10">
+        <v>509.85271164530002</v>
+      </c>
+      <c r="G154" s="10"/>
+      <c r="H154" s="10"/>
+      <c r="I154" s="10"/>
+      <c r="K154" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L154" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" s="10">
+        <v>509.24299473420001</v>
+      </c>
+      <c r="G155" s="10"/>
+      <c r="H155" s="10"/>
+      <c r="I155" s="10"/>
+      <c r="K155" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L155" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" s="10">
+        <v>508.83812695180001</v>
+      </c>
+      <c r="G156" s="10"/>
+      <c r="H156" s="10"/>
+      <c r="I156" s="10"/>
+      <c r="K156" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L156" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="10">
+        <v>508.66381229630002</v>
+      </c>
+      <c r="G157" s="10"/>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10"/>
+      <c r="K157" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L157" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" s="10">
+        <v>506.55305853930003</v>
+      </c>
+      <c r="G158" s="10"/>
+      <c r="H158" s="10"/>
+      <c r="I158" s="10"/>
+      <c r="K158" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L158" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="10">
+        <v>507.59767346439997</v>
+      </c>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
+      <c r="K159" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L159" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="10">
+        <v>507.72042552570002</v>
+      </c>
+      <c r="G160" s="10"/>
+      <c r="H160" s="10"/>
+      <c r="I160" s="10"/>
+      <c r="K160" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L160" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="10">
+        <v>509.51362790770003</v>
+      </c>
+      <c r="G161" s="10"/>
+      <c r="H161" s="10"/>
+      <c r="I161" s="10"/>
+      <c r="K161" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L161" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{846BE28D-8DCC-4D37-9121-69E2905DE42A}">
+      <formula1>$P$2:$P$4</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Enabled settings on Excel sheets (#6)
* Enabled settings on Excel sheets

* Bugfix for range of extrapolation and position of words
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7EDB14-C8D1-418D-9406-304F6E84B4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D973CBAE-49C3-4D01-8764-A8148534C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slot 1" sheetId="4" r:id="rId1"/>
-    <sheet name="Slot 2" sheetId="7" r:id="rId2"/>
+    <sheet name="Slot 2" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>site 7 n/a</t>
   </si>
@@ -77,12 +76,48 @@
   <si>
     <t>Plot 10</t>
   </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Wafer radius (mm)</t>
+  </si>
+  <si>
+    <t>Unit for X,Y coordinates</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>μm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Range of colorbar</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>(Range of colorbar entered should be larger than actual range of data values)</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Hi2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +131,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -113,15 +167,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,15 +308,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -180,8 +331,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8953500" y="66674"/>
-          <a:ext cx="3571875" cy="4067175"/>
+          <a:off x="8886825" y="971550"/>
+          <a:ext cx="3429000" cy="4305300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -440,7 +591,24 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Please create a new sheet for data from a different test slot.  You can do this by left clicking on a sheet name, and select "Move or Copy", then click "Create a copy" and "OK".</a:t>
+            <a:t>Please create a new sheet for data from a different test slot.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can do this by left clicking on a sheet name, and select "Move or Copy", then click "Create a copy" and "OK".</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -509,7 +677,565 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. If there's n filled columns in a Worksheet (excluding the last 2 columns containing coordinates), n images will be generated. The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can rename the columns in the first row and the new names will be used in image namings. </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687D2300-2B01-4D81-B092-1E5A5EF88834}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886825" y="981075"/>
+          <a:ext cx="3429000" cy="4305300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:shade val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Data input format</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Each set of data points for a plot should be inserted into individual columns.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The "X", "Y" columns should contain the coordinates of the datapoints. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> i.e. All data points in the same row should share the same coordinates. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please enter the X, Y coordinates with units mm.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please create a new sheet for data from a different test slot.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can do this by left clicking on a sheet name, and select "Move or Copy", then click "Create a copy" and "OK".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -586,30 +1312,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{24DAC0C6-B2EB-4124-A643-0F1E288FC213}" name="Table27" displayName="Table27" ref="A1:J55" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:J55" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{63EA718A-983D-431F-847B-6CE904B48EAC}" name="Table212" displayName="Table212" ref="A1:J161" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:J161" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CAAA24BB-705F-4A4B-A80A-FDB35DE069CD}" name="Plot 1"/>
-    <tableColumn id="2" xr3:uid="{A96A166F-7D26-454E-B9ED-96FD4C7DABD7}" name="Plot 2"/>
-    <tableColumn id="3" xr3:uid="{AF77A07D-DF4A-4686-9EE0-2E28C11ECB6D}" name="Plot 3"/>
-    <tableColumn id="4" xr3:uid="{3B8900D9-CC21-4E17-9A17-7B58BFC8D62E}" name="Plot 4"/>
-    <tableColumn id="5" xr3:uid="{B9D10A16-796B-4AA9-A260-DB9776871A2B}" name="Plot 5"/>
-    <tableColumn id="6" xr3:uid="{5E38E4B4-BC12-4BEE-80F6-FD6663B99283}" name="Plot 6"/>
-    <tableColumn id="7" xr3:uid="{8291302C-DA66-4347-939C-89EE191B3D5C}" name="Plot 7"/>
-    <tableColumn id="8" xr3:uid="{E61E32E9-2F11-496B-BEFA-5770A03AB077}" name="Plot 8"/>
-    <tableColumn id="9" xr3:uid="{78F822B7-7C80-4961-B7E3-5888420DAF66}" name="Plot 9"/>
-    <tableColumn id="10" xr3:uid="{300152D7-FD7A-463D-BA9D-810F6F2150FE}" name="Plot 10"/>
+    <tableColumn id="1" xr3:uid="{B06A5652-4273-45BF-B5E1-8E8EE2C4B32B}" name="Hi"/>
+    <tableColumn id="2" xr3:uid="{AC9C8AB1-8D4C-4FB4-8EFB-3C0184F0C16B}" name="Plot 2"/>
+    <tableColumn id="3" xr3:uid="{DBEB4D72-A830-463A-8A2F-D12D6BF6B954}" name="Plot 3"/>
+    <tableColumn id="4" xr3:uid="{509B5B0B-FE72-40C8-A074-F42BCBC3EE2D}" name="Plot 4"/>
+    <tableColumn id="5" xr3:uid="{BA5CC006-DF39-4A53-9C9B-3650A72E06DB}" name="Plot 5"/>
+    <tableColumn id="6" xr3:uid="{144A9648-C02B-468F-B296-61D208B3241A}" name="Hi2"/>
+    <tableColumn id="7" xr3:uid="{D0190320-FA9A-44B4-99C7-6D1805D13FBA}" name="Plot 7"/>
+    <tableColumn id="8" xr3:uid="{E8AEE2CA-A6D9-4BE1-9FBD-DE1F831CFECD}" name="Column1"/>
+    <tableColumn id="9" xr3:uid="{8E92826C-3BFC-4502-A174-037CED71E08E}" name="Column2"/>
+    <tableColumn id="10" xr3:uid="{DD1526E5-4B0D-4F05-98F4-066AC8B6F99D}" name="Plot 10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{64D710E8-1C44-435D-8059-F0BA971F6CC5}" name="Table38" displayName="Table38" ref="K1:L55" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="K1:L55" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8CBC8320-A488-46CA-AD26-836D2847824A}" name="Table313" displayName="Table313" ref="K1:L161" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="K1:L161" xr:uid="{63853220-0C14-4CDA-9C08-E9F5F768B780}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D07BFDB2-8B2A-435B-90CD-8A7F952C8846}" name="X"/>
-    <tableColumn id="2" xr3:uid="{02F4CF70-11D1-47DB-BFCB-A1379C51C00D}" name="Y"/>
+    <tableColumn id="1" xr3:uid="{970E6553-C0F1-4E98-9D12-24A80B3E2E54}" name="X"/>
+    <tableColumn id="2" xr3:uid="{A754B5EE-2228-40E5-B30B-7476D70FB60A}" name="Y"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -878,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC50625A-E453-4126-B67A-263A5ACC8F11}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,9 +1615,11 @@
     <col min="1" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="12" width="11" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -928,8 +1656,14 @@
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11862.2246</v>
       </c>
@@ -948,8 +1682,17 @@
       <c r="L2">
         <v>127.9237</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9975.8603999999996</v>
       </c>
@@ -968,8 +1711,17 @@
       <c r="L3">
         <v>5.9196</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11880.1602</v>
       </c>
@@ -988,8 +1740,14 @@
       <c r="L4">
         <v>103.52290000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11868.9521</v>
       </c>
@@ -1009,7 +1767,7 @@
         <v>5.9196</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11952.9072</v>
       </c>
@@ -1029,7 +1787,7 @@
         <v>-91.683700000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11997.059600000001</v>
       </c>
@@ -1049,7 +1807,7 @@
         <v>-116.08459999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12241.3613</v>
       </c>
@@ -1059,7 +1817,7 @@
       <c r="C8">
         <v>12856.838900000001</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K8">
@@ -1069,7 +1827,7 @@
         <v>-67.282899999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9811.4531000000006</v>
       </c>
@@ -1089,7 +1847,7 @@
         <v>5.9196</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9827.3271000000004</v>
       </c>
@@ -1109,7 +1867,7 @@
         <v>79.122100000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9925.7813000000006</v>
       </c>
@@ -1129,7 +1887,7 @@
         <v>79.122100000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9848.6288999999997</v>
       </c>
@@ -1149,7 +1907,7 @@
         <v>30.320399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9650.8583999999992</v>
       </c>
@@ -1169,7 +1927,7 @@
         <v>-42.882100000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9936.4267999999993</v>
       </c>
@@ -1189,7 +1947,7 @@
         <v>-42.882100000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9930.7304999999997</v>
       </c>
@@ -1211,6 +1969,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{FB4092C1-549A-440B-ABF8-D4591512FD6B}">
+      <formula1>$P$2:$P$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1222,11 +1985,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA81F29-FE7A-42C0-BA49-A436353A8637}">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58ADF574-3877-422C-9DBE-63782FDF5636}">
+  <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,11 +1997,13 @@
     <col min="1" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="12" width="11" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -1253,16 +2018,16 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -1273,14 +2038,2290 @@
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>508.36828172640003</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="K2" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L2" s="10">
+        <v>135074.34619140599</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>506.46913551149999</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L3" s="10">
+        <v>135074.34619140599</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>507.49098546720001</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="K4" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L4" s="10">
+        <v>135074.34619140599</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>507.94784226019999</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="K5" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L5" s="10">
+        <v>135074.34619140599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>506.14143917720003</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="K6" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L6" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>506.2219809211</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="K7" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L7" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>506.14198926080002</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="K8" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L8" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>506.3368160425</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="K9" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L9" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>507.67092865030003</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="K10" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L10" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>508.06090553090002</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="K11" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L11" s="10">
+        <v>119204.346191406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>507.65969628959999</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="K12" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L12" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>507.19103347629999</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="K13" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L13" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>506.21199639129998</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="K14" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L14" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>503.53583453260001</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="K15" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L15" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>505.1798968718</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="K16" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L16" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>504.55994906519999</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="K17" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L17" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>504.68103425919998</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="K18" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L18" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>505.2765473856</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="K19" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L19" s="10">
+        <v>103334.346191406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>507.39221471899998</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="K20" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L20" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>505.68590665440001</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="K21" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L21" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>505.60833122410003</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="K22" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L22" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>507.05780156740002</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="K23" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L23" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>505.36023726989998</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="K24" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L24" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>507.29234123930001</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="K25" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L25" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>505.76881296720001</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="K26" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L26" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>507.7906963634</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="K27" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L27" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>509.83305878469997</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="K28" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L28" s="10">
+        <v>87464.346191406206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>508.30575559120001</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="K29" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L29" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>505.8527186</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="K30" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L30" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>506.35430825050003</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="K31" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L31" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>507.41795592030002</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="K32" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L32" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>506.59827754510002</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="K33" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L33" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>506.7303448545</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="K34" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L34" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>506.38634828630001</v>
+      </c>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="K35" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L35" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>508.06075160419999</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="K36" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L36" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>507.14301376660001</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="K37" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L37" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>506.08612143760001</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="K38" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L38" s="10">
+        <v>71594.346191406206</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>504.99640320370003</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="K39" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L39" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>506.51909067150001</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="K40" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L40" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>507.4010398561</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="K41" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L41" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>505.57609722929999</v>
+      </c>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="K42" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L42" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>507.04529497419998</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="K43" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L43" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>503.82989180089999</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="K44" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L44" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>504.83838626570002</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="K45" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L45" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>506.70121251130001</v>
+      </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="K46" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L46" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>505.30617168139997</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="K47" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L47" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>508.70395182750002</v>
+      </c>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="K48" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L48" s="10">
+        <v>55724.346191406199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>508.27752415650002</v>
+      </c>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="K49" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L49" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>507.97805429879998</v>
+      </c>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="K50" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L50" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>507.23137949210002</v>
+      </c>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="K51" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L51" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>505.83747482929999</v>
+      </c>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="K52" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L52" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>505.23275112610003</v>
+      </c>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="K53" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L53" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>505.55489078940002</v>
+      </c>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="K54" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L54" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
+        <v>505.75672325699998</v>
+      </c>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="K55" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L55" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>507.46174422489997</v>
+      </c>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="K56" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L56" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="10">
+        <v>505.7781708393</v>
+      </c>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="K57" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L57" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="10">
+        <v>506.29255188669998</v>
+      </c>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="K58" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L58" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>507.40917216000003</v>
+      </c>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="K59" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L59" s="10">
+        <v>39854.346191406199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="10">
+        <v>507.36214164030002</v>
+      </c>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="K60" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L60" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="10">
+        <v>505.94454003829998</v>
+      </c>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="K61" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L61" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="10">
+        <v>506.26983902069998</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="K62" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L62" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
+        <v>505.38198615990001</v>
+      </c>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="K63" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L63" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="10">
+        <v>506.81426540730001</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="K64" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L64" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="10">
+        <v>505.4120314443</v>
+      </c>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="K65" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L65" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="10">
+        <v>506.89331163589998</v>
+      </c>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="K66" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L66" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="10">
+        <v>506.88526217560002</v>
+      </c>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="K67" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L67" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="10">
+        <v>508.39181327239999</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="K68" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L68" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="10">
+        <v>508.32606564060001</v>
+      </c>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="K69" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L69" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="10">
+        <v>509.49072453180003</v>
+      </c>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="K70" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L70" s="10">
+        <v>23984.346191406199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="10">
+        <v>511.11256765740001</v>
+      </c>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="K71" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L71" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="10">
+        <v>507.56900084680001</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="K72" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L72" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="10">
+        <v>507.42683955669997</v>
+      </c>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="K73" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L73" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
+        <v>507.05576994</v>
+      </c>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="K74" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L74" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
+        <v>507.44634169</v>
+      </c>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="K75" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L75" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="10">
+        <v>507.53114358459999</v>
+      </c>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="K76" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L76" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="10">
+        <v>506.8724407986</v>
+      </c>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="K77" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L77" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
+        <v>507.06825752809999</v>
+      </c>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="K78" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L78" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="10">
+        <v>506.85195381509999</v>
+      </c>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="K79" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L79" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="10">
+        <v>506.26778247919998</v>
+      </c>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="K80" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L80" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="10">
+        <v>506.53828329100003</v>
+      </c>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="K81" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L81" s="10">
+        <v>8114.3461914062</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>507.90198703829998</v>
+      </c>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="K82" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L82" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="10">
+        <v>506.62476672420001</v>
+      </c>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="K83" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L83" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="10">
+        <v>507.40631653849999</v>
+      </c>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="K84" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L84" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="10">
+        <v>508.0877120376</v>
+      </c>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="K85" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L85" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="10">
+        <v>507.14928302499999</v>
+      </c>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="K86" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L86" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="10">
+        <v>508.1512023107</v>
+      </c>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="K87" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L87" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="10">
+        <v>507.4980302372</v>
+      </c>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="K88" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L88" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="10">
+        <v>508.28363662729998</v>
+      </c>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="K89" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L89" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="10">
+        <v>507.50816252689998</v>
+      </c>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="K90" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L90" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="10">
+        <v>507.62666497409998</v>
+      </c>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="K91" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L91" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="10">
+        <v>507.62669499899999</v>
+      </c>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="K92" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L92" s="10">
+        <v>-7755.6538085937</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="10">
+        <v>508.87112796500003</v>
+      </c>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="K93" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L93" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="10">
+        <v>507.06661210009997</v>
+      </c>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="K94" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L94" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="10">
+        <v>507.6134279858</v>
+      </c>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="K95" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L95" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="10">
+        <v>507.13697527839997</v>
+      </c>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="K96" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L96" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="10">
+        <v>507.60699275809998</v>
+      </c>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="K97" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L97" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="10">
+        <v>507.95306041600003</v>
+      </c>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="K98" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L98" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="10">
+        <v>507.795266368</v>
+      </c>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="K99" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L99" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="10">
+        <v>507.25245776179997</v>
+      </c>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="K100" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L100" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="10">
+        <v>506.99316613830001</v>
+      </c>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="K101" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L101" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="10">
+        <v>507.46517910159997</v>
+      </c>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+      <c r="I102" s="10"/>
+      <c r="K102" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L102" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="10">
+        <v>507.89433567740002</v>
+      </c>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="K103" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L103" s="10">
+        <v>-23625.653808593801</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="10">
+        <v>507.40430452610002</v>
+      </c>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="K104" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L104" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="10">
+        <v>506.73101552740002</v>
+      </c>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="K105" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L105" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="10">
+        <v>506.36912536009999</v>
+      </c>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="K106" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L106" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="10">
+        <v>507.10280864660001</v>
+      </c>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="K107" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L107" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108" s="10">
+        <v>505.29861237350002</v>
+      </c>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="K108" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L108" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" s="10">
+        <v>506.6675904544</v>
+      </c>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="K109" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L109" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" s="10">
+        <v>506.68239760469999</v>
+      </c>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+      <c r="K110" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L110" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="10">
+        <v>505.79287174669997</v>
+      </c>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="K111" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L111" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" s="10">
+        <v>506.20664817890002</v>
+      </c>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="K112" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L112" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="10">
+        <v>506.70521801479998</v>
+      </c>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
+      <c r="I113" s="10"/>
+      <c r="K113" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L113" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="10">
+        <v>508.84779533059998</v>
+      </c>
+      <c r="G114" s="10"/>
+      <c r="H114" s="10"/>
+      <c r="I114" s="10"/>
+      <c r="K114" s="10">
+        <v>-142294.53417968799</v>
+      </c>
+      <c r="L114" s="10">
+        <v>-39495.653808593801</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="10">
+        <v>508.86391012370001</v>
+      </c>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="K115" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L115" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="10">
+        <v>507.27215344849998</v>
+      </c>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
+      <c r="I116" s="10"/>
+      <c r="K116" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L116" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="10">
+        <v>506.39187865129998</v>
+      </c>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+      <c r="K117" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L117" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="10">
+        <v>507.10705694059999</v>
+      </c>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+      <c r="I118" s="10"/>
+      <c r="K118" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L118" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="10">
+        <v>507.69632012770001</v>
+      </c>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+      <c r="I119" s="10"/>
+      <c r="K119" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L119" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="10">
+        <v>506.62663214460002</v>
+      </c>
+      <c r="G120" s="10"/>
+      <c r="H120" s="10"/>
+      <c r="I120" s="10"/>
+      <c r="K120" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L120" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="10">
+        <v>506.06629126849998</v>
+      </c>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+      <c r="K121" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L121" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" s="10">
+        <v>507.42915641180002</v>
+      </c>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="K122" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L122" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="10">
+        <v>506.60776187900001</v>
+      </c>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="K123" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L123" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="10">
+        <v>509.18979865649999</v>
+      </c>
+      <c r="G124" s="10"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="K124" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L124" s="10">
+        <v>-55365.653808593801</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="10">
+        <v>508.85556336209999</v>
+      </c>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="K125" s="10">
+        <v>117505.46582031201</v>
+      </c>
+      <c r="L125" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" s="10">
+        <v>508.9222274828</v>
+      </c>
+      <c r="G126" s="10"/>
+      <c r="H126" s="10"/>
+      <c r="I126" s="10"/>
+      <c r="K126" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L126" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="10">
+        <v>507.32045756999997</v>
+      </c>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="K127" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L127" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="10">
+        <v>508.67007377610003</v>
+      </c>
+      <c r="G128" s="10"/>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+      <c r="K128" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L128" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="10">
+        <v>507.69189612240001</v>
+      </c>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="K129" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L129" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" s="10">
+        <v>504.3425767448</v>
+      </c>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+      <c r="K130" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L130" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="10">
+        <v>507.48012327729998</v>
+      </c>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="K131" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L131" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="10">
+        <v>507.13903611770002</v>
+      </c>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="K132" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L132" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133" s="10">
+        <v>507.72222661759997</v>
+      </c>
+      <c r="G133" s="10"/>
+      <c r="H133" s="10"/>
+      <c r="I133" s="10"/>
+      <c r="K133" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L133" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="10">
+        <v>509.37322456700002</v>
+      </c>
+      <c r="G134" s="10"/>
+      <c r="H134" s="10"/>
+      <c r="I134" s="10"/>
+      <c r="K134" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L134" s="10">
+        <v>-71235.653808593794</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" s="10">
+        <v>508.61913568940003</v>
+      </c>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+      <c r="K135" s="10">
+        <v>-116314.53417968799</v>
+      </c>
+      <c r="L135" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="10">
+        <v>507.84549219759998</v>
+      </c>
+      <c r="G136" s="10"/>
+      <c r="H136" s="10"/>
+      <c r="I136" s="10"/>
+      <c r="K136" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L136" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="10">
+        <v>506.7125765111</v>
+      </c>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+      <c r="K137" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L137" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138" s="10">
+        <v>508.23058244020001</v>
+      </c>
+      <c r="G138" s="10"/>
+      <c r="H138" s="10"/>
+      <c r="I138" s="10"/>
+      <c r="K138" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L138" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" s="10">
+        <v>506.82398959480003</v>
+      </c>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+      <c r="K139" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L139" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="10">
+        <v>509.10760069690002</v>
+      </c>
+      <c r="G140" s="10"/>
+      <c r="H140" s="10"/>
+      <c r="I140" s="10"/>
+      <c r="K140" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L140" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" s="10">
+        <v>507.20794061459998</v>
+      </c>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
+      <c r="K141" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L141" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="10">
+        <v>508.90399061120002</v>
+      </c>
+      <c r="G142" s="10"/>
+      <c r="H142" s="10"/>
+      <c r="I142" s="10"/>
+      <c r="K142" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L142" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="10">
+        <v>508.4898106018</v>
+      </c>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+      <c r="K143" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L143" s="10">
+        <v>-87105.653808593794</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" s="10">
+        <v>507.23381260849999</v>
+      </c>
+      <c r="G144" s="10"/>
+      <c r="H144" s="10"/>
+      <c r="I144" s="10"/>
+      <c r="K144" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L144" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" s="10">
+        <v>506.89998225990001</v>
+      </c>
+      <c r="G145" s="10"/>
+      <c r="H145" s="10"/>
+      <c r="I145" s="10"/>
+      <c r="K145" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L145" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" s="10">
+        <v>507.9829626216</v>
+      </c>
+      <c r="G146" s="10"/>
+      <c r="H146" s="10"/>
+      <c r="I146" s="10"/>
+      <c r="K146" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L146" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="10">
+        <v>506.72239559100001</v>
+      </c>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+      <c r="K147" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L147" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" s="10">
+        <v>507.12327032979999</v>
+      </c>
+      <c r="G148" s="10"/>
+      <c r="H148" s="10"/>
+      <c r="I148" s="10"/>
+      <c r="K148" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L148" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" s="10">
+        <v>506.22694080259998</v>
+      </c>
+      <c r="G149" s="10"/>
+      <c r="H149" s="10"/>
+      <c r="I149" s="10"/>
+      <c r="K149" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L149" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" s="10">
+        <v>508.38049034779999</v>
+      </c>
+      <c r="G150" s="10"/>
+      <c r="H150" s="10"/>
+      <c r="I150" s="10"/>
+      <c r="K150" s="10">
+        <v>-90334.5341796875</v>
+      </c>
+      <c r="L150" s="10">
+        <v>-102975.653808594</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" s="10">
+        <v>508.51205468609999</v>
+      </c>
+      <c r="G151" s="10"/>
+      <c r="H151" s="10"/>
+      <c r="I151" s="10"/>
+      <c r="K151" s="10">
+        <v>-64354.5341796875</v>
+      </c>
+      <c r="L151" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152" s="10">
+        <v>507.4783165019</v>
+      </c>
+      <c r="G152" s="10"/>
+      <c r="H152" s="10"/>
+      <c r="I152" s="10"/>
+      <c r="K152" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L152" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A153" s="10">
+        <v>508.47489269149997</v>
+      </c>
+      <c r="G153" s="10"/>
+      <c r="H153" s="10"/>
+      <c r="I153" s="10"/>
+      <c r="K153" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L153" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A154" s="10">
+        <v>509.85271164530002</v>
+      </c>
+      <c r="G154" s="10"/>
+      <c r="H154" s="10"/>
+      <c r="I154" s="10"/>
+      <c r="K154" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L154" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" s="10">
+        <v>509.24299473420001</v>
+      </c>
+      <c r="G155" s="10"/>
+      <c r="H155" s="10"/>
+      <c r="I155" s="10"/>
+      <c r="K155" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L155" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" s="10">
+        <v>508.83812695180001</v>
+      </c>
+      <c r="G156" s="10"/>
+      <c r="H156" s="10"/>
+      <c r="I156" s="10"/>
+      <c r="K156" s="10">
+        <v>65545.4658203125</v>
+      </c>
+      <c r="L156" s="10">
+        <v>-118845.653808594</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="10">
+        <v>508.66381229630002</v>
+      </c>
+      <c r="G157" s="10"/>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10"/>
+      <c r="K157" s="10">
+        <v>39565.4658203125</v>
+      </c>
+      <c r="L157" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" s="10">
+        <v>506.55305853930003</v>
+      </c>
+      <c r="G158" s="10"/>
+      <c r="H158" s="10"/>
+      <c r="I158" s="10"/>
+      <c r="K158" s="10">
+        <v>13585.4658203125</v>
+      </c>
+      <c r="L158" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="10">
+        <v>507.59767346439997</v>
+      </c>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
+      <c r="K159" s="10">
+        <v>-12394.5341796875</v>
+      </c>
+      <c r="L159" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="10">
+        <v>507.72042552570002</v>
+      </c>
+      <c r="G160" s="10"/>
+      <c r="H160" s="10"/>
+      <c r="I160" s="10"/>
+      <c r="K160" s="10">
+        <v>-38374.5341796875</v>
+      </c>
+      <c r="L160" s="10">
+        <v>-134715.65380859401</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="10">
+        <v>509.51362790770003</v>
+      </c>
+      <c r="G161" s="10"/>
+      <c r="H161" s="10"/>
+      <c r="I161" s="10"/>
+      <c r="K161" s="10">
+        <v>91525.4658203125</v>
+      </c>
+      <c r="L161" s="10">
+        <v>-102975.653808594</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{846BE28D-8DCC-4D37-9121-69E2905DE42A}">
+      <formula1>$P$2:$P$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
min max for colorbar implemented in excel
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B545DC-7C50-489F-AFC1-21C9DFC1F0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5095B731-A548-4EC0-9C50-609494A84978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Y</t>
   </si>
@@ -88,23 +88,26 @@
     <t>cm</t>
   </si>
   <si>
-    <t>Range of colorbar</t>
-  </si>
-  <si>
-    <t>(Range of colorbar entered should be larger than actual range of data values)</t>
-  </si>
-  <si>
     <t>Auto</t>
   </si>
   <si>
-    <t>(For range to be auto enter "Auto" or just leave blank)</t>
+    <t>(Min/max of colorbar entered should cover actual range of data values)</t>
+  </si>
+  <si>
+    <t>(For min/max to be auto enter "Auto" or just leave blank)</t>
+  </si>
+  <si>
+    <t>Colobar Min</t>
+  </si>
+  <si>
+    <t>Colobar Max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +118,13 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -168,32 +178,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color theme="9"/>
       </top>
@@ -210,9 +194,7 @@
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -220,9 +202,36 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color theme="9"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -232,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -241,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,7 +259,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,16 +289,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -302,8 +313,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8886825" y="981075"/>
-          <a:ext cx="3429000" cy="4305300"/>
+          <a:off x="9486899" y="1171576"/>
+          <a:ext cx="3057525" cy="3752850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -461,40 +472,20 @@
             </a:rPr>
             <a:t>The "X", "Y" columns should contain the coordinates of the datapoints. </a:t>
           </a:r>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> i.e. All data points in the same row should share the same coordinates. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Please enter the X, Y coordinates with units mm.</a:t>
-          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -648,7 +639,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. Plots produced could be found under the "Images" folder. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -717,7 +708,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
+            <a:t>The naming of images will be of the format "Spreadsheet name_Column name" </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -766,6 +757,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{01DEE21E-09A8-4CAC-ACED-A15C3ACF767E}" name="Table268" displayName="Table268" ref="A1:J161" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:J161" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J15">
+    <sortCondition ref="A2:A15"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9E9E73E0-482E-4A4D-AD3D-79B9F714F90F}" name="Plot 1"/>
     <tableColumn id="2" xr3:uid="{D149ABE7-A8FD-4C2A-8C36-517E1D897314}" name="Plot 2"/>
@@ -1056,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B65AA46-2D62-48F7-8C24-BD2CA98A6564}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,44 +1105,112 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="8">
         <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N2" s="4" t="s">
+      <c r="A2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N3" s="6" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="P3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N4" s="8" t="s">
-        <v>18</v>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="N4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="P4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N5" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
min max for colorbar implemented in excel (#7)
</commit_message>
<xml_diff>
--- a/main/data.xlsx
+++ b/main/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu-cjk\Desktop\wafer_thickness_tool\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B545DC-7C50-489F-AFC1-21C9DFC1F0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5095B731-A548-4EC0-9C50-609494A84978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Y</t>
   </si>
@@ -88,23 +88,26 @@
     <t>cm</t>
   </si>
   <si>
-    <t>Range of colorbar</t>
-  </si>
-  <si>
-    <t>(Range of colorbar entered should be larger than actual range of data values)</t>
-  </si>
-  <si>
     <t>Auto</t>
   </si>
   <si>
-    <t>(For range to be auto enter "Auto" or just leave blank)</t>
+    <t>(Min/max of colorbar entered should cover actual range of data values)</t>
+  </si>
+  <si>
+    <t>(For min/max to be auto enter "Auto" or just leave blank)</t>
+  </si>
+  <si>
+    <t>Colobar Min</t>
+  </si>
+  <si>
+    <t>Colobar Max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +118,13 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -168,32 +178,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color theme="9"/>
       </top>
@@ -210,9 +194,7 @@
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -220,9 +202,36 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color theme="9"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -232,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -241,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,7 +259,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,16 +289,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -302,8 +313,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8886825" y="981075"/>
-          <a:ext cx="3429000" cy="4305300"/>
+          <a:off x="9486899" y="1171576"/>
+          <a:ext cx="3057525" cy="3752850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -461,40 +472,20 @@
             </a:rPr>
             <a:t>The "X", "Y" columns should contain the coordinates of the datapoints. </a:t>
           </a:r>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> i.e. All data points in the same row should share the same coordinates. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="sng" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Please enter the X, Y coordinates with units mm.</a:t>
-          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-SG" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -648,7 +639,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. After the terminal prompts that the program has completed, plots produced could be found under the "Images" folder. </a:t>
+            <a:t>After insertion of data, proceed to the same folder containing the current Excel file to find the "wafer_thickness_tool.bat" file. Double click to start the program. Plots produced could be found under the "Images" folder. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -717,7 +708,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The naming of the images will be of the format "Spreadsheet name_Column name" E.g. Data under "Plot 1" of Slot 1 will be named "Slot 1_Plot 1.png"</a:t>
+            <a:t>The naming of images will be of the format "Spreadsheet name_Column name" </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -766,6 +757,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{01DEE21E-09A8-4CAC-ACED-A15C3ACF767E}" name="Table268" displayName="Table268" ref="A1:J161" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:J161" xr:uid="{422048D9-A6C0-4922-A0C4-44B0A5EC4B6E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J15">
+    <sortCondition ref="A2:A15"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9E9E73E0-482E-4A4D-AD3D-79B9F714F90F}" name="Plot 1"/>
     <tableColumn id="2" xr3:uid="{D149ABE7-A8FD-4C2A-8C36-517E1D897314}" name="Plot 2"/>
@@ -1056,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B65AA46-2D62-48F7-8C24-BD2CA98A6564}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,44 +1105,112 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="8">
         <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N2" s="4" t="s">
+      <c r="A2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N3" s="6" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="P3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N4" s="8" t="s">
-        <v>18</v>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="N4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="P4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N5" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>